<commit_message>
Cambios por USFQ/UCR (1).
</commit_message>
<xml_diff>
--- a/AgriculturaUSCUSS/Model/2_Model/BAU/ModeloSuelo_BAU.xlsx
+++ b/AgriculturaUSCUSS/Model/2_Model/BAU/ModeloSuelo_BAU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaman\OneDrive\Escritorio\1_AFOLU\2_Model\BAU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/677db98c2725c13a/Escritorio/1_AFOLU/2_Model/BAU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABAD960-A55E-44A4-A88D-7EAA0AB0D52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{CABAD960-A55E-44A4-A88D-7EAA0AB0D52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8DF32CA4-0BE7-4C1E-8563-5C461FFE891E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="18" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Content" sheetId="13" r:id="rId1"/>
@@ -1970,6 +1970,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2438,8 +2442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:BO22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M22"/>
+    <sheetView topLeftCell="AO1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20:BN20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6151,7 +6155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:BO58"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AT40" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M58" sqref="M3:M58"/>
     </sheetView>
   </sheetViews>
@@ -30108,8 +30112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:BO88"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M88" sqref="M3:M88"/>
+    <sheetView topLeftCell="AU70" zoomScale="96" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BJ88" sqref="BJ88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -43489,154 +43493,154 @@
         <v>8.0239179269296676E-2</v>
       </c>
       <c r="Q76">
-        <v>7.9309315543439771E-2</v>
+        <v>8.1185485842081073E-2</v>
       </c>
       <c r="R76">
-        <v>8.0683258449938886E-2</v>
+        <v>8.1750582031237098E-2</v>
       </c>
       <c r="S76">
-        <v>8.2024978831346698E-2</v>
+        <v>8.1750582031237098E-2</v>
       </c>
       <c r="T76">
-        <v>8.3169946042576451E-2</v>
+        <v>8.1767613402493583E-2</v>
       </c>
       <c r="U76">
-        <v>8.4025965524722565E-2</v>
+        <v>8.1784644773750109E-2</v>
       </c>
       <c r="V76">
-        <v>8.5649478677154708E-2</v>
+        <v>8.1801676145006594E-2</v>
       </c>
       <c r="W76">
-        <v>8.7042322591276824E-2</v>
+        <v>8.1818707516263106E-2</v>
       </c>
       <c r="X76">
-        <v>8.7923342220835574E-2</v>
+        <v>8.1835738887519605E-2</v>
       </c>
       <c r="Y76">
-        <v>8.899946176950764E-2</v>
+        <v>8.1852770258776089E-2</v>
       </c>
       <c r="Z76">
-        <v>9.0805593306509405E-2</v>
+        <v>8.1869801630032601E-2</v>
       </c>
       <c r="AA76">
-        <v>9.2044470939765338E-2</v>
+        <v>8.1886833001289114E-2</v>
       </c>
       <c r="AB76">
-        <v>9.3712865697144668E-2</v>
+        <v>8.1903864372545626E-2</v>
       </c>
       <c r="AC76">
-        <v>9.4951344981748453E-2</v>
+        <v>8.1920895743802125E-2</v>
       </c>
       <c r="AD76">
-        <v>9.6230641263276823E-2</v>
+        <v>8.1937927115058623E-2</v>
       </c>
       <c r="AE76">
-        <v>9.7734492211623489E-2</v>
+        <v>8.1954958486315135E-2</v>
       </c>
       <c r="AF76">
-        <v>9.9013327377753868E-2</v>
+        <v>8.1971989857571634E-2</v>
       </c>
       <c r="AG76">
-        <v>0.100408564247651</v>
+        <v>8.1989021228828132E-2</v>
       </c>
       <c r="AH76">
-        <v>0.10202853839957503</v>
+        <v>8.2006052600084645E-2</v>
       </c>
       <c r="AI76">
-        <v>0.10345011521344678</v>
+        <v>8.2023083971341157E-2</v>
       </c>
       <c r="AJ76">
-        <v>0.10493095967306955</v>
+        <v>8.2040115342597655E-2</v>
       </c>
       <c r="AK76">
-        <v>0.10640423489545826</v>
+        <v>8.2057146713854168E-2</v>
       </c>
       <c r="AL76">
-        <v>0.1074207003367549</v>
+        <v>8.207417808511068E-2</v>
       </c>
       <c r="AM76">
-        <v>0.10894653727920528</v>
+        <v>8.2091209456367165E-2</v>
       </c>
       <c r="AN76">
-        <v>0.11016246586132591</v>
+        <v>8.2108240827623677E-2</v>
       </c>
       <c r="AO76">
-        <v>0.11188739959629587</v>
+        <v>8.2125272198880162E-2</v>
       </c>
       <c r="AP76">
-        <v>0.11317536269490452</v>
+        <v>8.214230357013666E-2</v>
       </c>
       <c r="AQ76">
-        <v>0.11444872622566717</v>
+        <v>8.21593349413932E-2</v>
       </c>
       <c r="AR76">
-        <v>0.11580271994085486</v>
+        <v>8.2176366312649698E-2</v>
       </c>
       <c r="AS76">
-        <v>0.11717853550830594</v>
+        <v>8.2193397683906197E-2</v>
       </c>
       <c r="AT76">
-        <v>0.11649446892829167</v>
+        <v>8.2210429055162695E-2</v>
       </c>
       <c r="AU76">
-        <v>0.11817436870488254</v>
+        <v>8.2227460426419194E-2</v>
       </c>
       <c r="AV76">
-        <v>0.1196531520913756</v>
+        <v>8.2244491797675706E-2</v>
       </c>
       <c r="AW76">
-        <v>0.12114197299799988</v>
+        <v>8.2261523168932218E-2</v>
       </c>
       <c r="AX76">
-        <v>0.12270823332277579</v>
+        <v>8.2278554540188717E-2</v>
       </c>
       <c r="AY76">
-        <v>0.12430523817630963</v>
+        <v>8.2295585911445215E-2</v>
       </c>
       <c r="AZ76">
-        <v>0.1259736438600538</v>
+        <v>8.2312617282701728E-2</v>
       </c>
       <c r="BA76">
-        <v>0.1275852188567978</v>
+        <v>8.2329648653958226E-2</v>
       </c>
       <c r="BB76">
-        <v>0.12923166363673286</v>
+        <v>8.2346680025214739E-2</v>
       </c>
       <c r="BC76">
-        <v>0.13091314810157478</v>
+        <v>8.2363711396471237E-2</v>
       </c>
       <c r="BD76">
-        <v>0.13262088305904687</v>
+        <v>8.2380742767727749E-2</v>
       </c>
       <c r="BE76">
-        <v>0.13434692643731153</v>
+        <v>8.2397774138984262E-2</v>
       </c>
       <c r="BF76">
-        <v>0.13609817978830643</v>
+        <v>8.241480551024076E-2</v>
       </c>
       <c r="BG76">
-        <v>0.13787804285813191</v>
+        <v>8.2431836881497259E-2</v>
       </c>
       <c r="BH76">
-        <v>0.13968807658220733</v>
+        <v>8.2448868252753771E-2</v>
       </c>
       <c r="BI76">
-        <v>0.14152333587262683</v>
+        <v>8.2465899624010283E-2</v>
       </c>
       <c r="BJ76">
-        <v>0.14338458038195448</v>
+        <v>8.2482930995266768E-2</v>
       </c>
       <c r="BK76">
-        <v>0.14527009036538968</v>
+        <v>8.2499962366523266E-2</v>
       </c>
       <c r="BL76">
-        <v>0.14718537203616028</v>
+        <v>8.2516993737779779E-2</v>
       </c>
       <c r="BM76">
-        <v>0.14913005138061292</v>
+        <v>8.2534025109036263E-2</v>
       </c>
       <c r="BN76">
-        <v>0.15110386308561247</v>
+        <v>8.2551056480292775E-2</v>
       </c>
     </row>
     <row r="77" spans="1:66" x14ac:dyDescent="0.3">
@@ -43668,154 +43672,154 @@
         <v>0.61444425538351022</v>
       </c>
       <c r="Q77">
-        <v>0.60732367626187278</v>
+        <v>0.65387949155775271</v>
       </c>
       <c r="R77">
-        <v>0.61784486221879753</v>
+        <v>0.65478006958333956</v>
       </c>
       <c r="S77">
-        <v>0.62811929907364294</v>
+        <v>0.65614419472830487</v>
       </c>
       <c r="T77">
-        <v>0.63688706728798961</v>
+        <v>0.65750831987327019</v>
       </c>
       <c r="U77">
-        <v>0.64344217238865087</v>
+        <v>0.65887244501823539</v>
       </c>
       <c r="V77">
-        <v>0.65587448212980015</v>
+        <v>0.66023657016320048</v>
       </c>
       <c r="W77">
-        <v>0.66654040555364169</v>
+        <v>0.66160069530816601</v>
       </c>
       <c r="X77">
-        <v>0.67328695325256138</v>
+        <v>0.66296482045313132</v>
       </c>
       <c r="Y77">
-        <v>0.68152750955945351</v>
+        <v>0.66432894559809641</v>
       </c>
       <c r="Z77">
-        <v>0.69535824857602735</v>
+        <v>0.66569307074306172</v>
       </c>
       <c r="AA77">
-        <v>0.70484515075784593</v>
+        <v>0.66705719588802692</v>
       </c>
       <c r="AB77">
-        <v>0.71762114851504077</v>
+        <v>0.66842132103299223</v>
       </c>
       <c r="AC77">
-        <v>0.72710500027880698</v>
+        <v>0.66978544617795754</v>
       </c>
       <c r="AD77">
-        <v>0.73690141467731995</v>
+        <v>0.67114957132292263</v>
       </c>
       <c r="AE77">
-        <v>0.74841739209108982</v>
+        <v>0.67251369646788817</v>
       </c>
       <c r="AF77">
-        <v>0.75821027542522801</v>
+        <v>0.67387782161285337</v>
       </c>
       <c r="AG77">
-        <v>0.76889452328786301</v>
+        <v>0.67524194675781846</v>
       </c>
       <c r="AH77">
-        <v>0.78129973257070973</v>
+        <v>0.67660607190278366</v>
       </c>
       <c r="AI77">
-        <v>0.79218568273650525</v>
+        <v>0.67797019704774886</v>
       </c>
       <c r="AJ77">
-        <v>0.80352548430997273</v>
+        <v>0.67933432219271406</v>
       </c>
       <c r="AK77">
-        <v>0.81480732324750038</v>
+        <v>0.68069844733767948</v>
       </c>
       <c r="AL77">
-        <v>0.82259106875547028</v>
+        <v>0.68206257248264479</v>
       </c>
       <c r="AM77">
-        <v>0.83427540740995754</v>
+        <v>0.68342669762760999</v>
       </c>
       <c r="AN77">
-        <v>0.84358657358892808</v>
+        <v>0.68479082277257519</v>
       </c>
       <c r="AO77">
-        <v>0.85679552754410737</v>
+        <v>0.68615494791754039</v>
       </c>
       <c r="AP77">
-        <v>0.86665830947050304</v>
+        <v>0.6875190730625057</v>
       </c>
       <c r="AQ77">
-        <v>0.87640929288804337</v>
+        <v>0.68888319820747113</v>
       </c>
       <c r="AR77">
-        <v>0.88677771474503031</v>
+        <v>0.69024732335243633</v>
       </c>
       <c r="AS77">
-        <v>0.89731324090053011</v>
+        <v>0.69161144849740142</v>
       </c>
       <c r="AT77">
-        <v>0.89207489245009364</v>
+        <v>0.69297557364236695</v>
       </c>
       <c r="AU77">
-        <v>0.90493899171863235</v>
+        <v>0.69433969878733215</v>
       </c>
       <c r="AV77">
-        <v>0.91626301029735824</v>
+        <v>0.69570382393229746</v>
       </c>
       <c r="AW77">
-        <v>0.92766389278021533</v>
+        <v>0.69706794907726277</v>
       </c>
       <c r="AX77">
-        <v>0.93965777990316013</v>
+        <v>0.69843207422222786</v>
       </c>
       <c r="AY77">
-        <v>0.95188709813658989</v>
+        <v>0.69979619936719339</v>
       </c>
       <c r="AZ77">
-        <v>0.96466317956415848</v>
+        <v>0.70116032451215859</v>
       </c>
       <c r="BA77">
-        <v>0.97700407098262232</v>
+        <v>0.7025244496571238</v>
       </c>
       <c r="BB77">
-        <v>0.98961198330238809</v>
+        <v>0.703888574802089</v>
       </c>
       <c r="BC77">
-        <v>1.0024882175728214</v>
+        <v>0.7052526999470542</v>
       </c>
       <c r="BD77">
-        <v>1.0155654691585418</v>
+        <v>0.70661682509201951</v>
       </c>
       <c r="BE77">
-        <v>1.028782920383436</v>
+        <v>0.70798095023698493</v>
       </c>
       <c r="BF77">
-        <v>1.0421934209772736</v>
+        <v>0.70934507538195013</v>
       </c>
       <c r="BG77">
-        <v>1.055823005035619</v>
+        <v>0.71070920052691544</v>
       </c>
       <c r="BH77">
-        <v>1.0696836256692865</v>
+        <v>0.71207332567188086</v>
       </c>
       <c r="BI77">
-        <v>1.0837374150824712</v>
+        <v>0.71343745081684629</v>
       </c>
       <c r="BJ77">
-        <v>1.0979901904352982</v>
+        <v>0.71480157596181138</v>
       </c>
       <c r="BK77">
-        <v>1.1124287825089003</v>
+        <v>0.71616570110677646</v>
       </c>
       <c r="BL77">
-        <v>1.1270953560053301</v>
+        <v>0.71752982625174189</v>
       </c>
       <c r="BM77">
-        <v>1.1419870468556512</v>
+        <v>0.71889395139670709</v>
       </c>
       <c r="BN77">
-        <v>1.1571018233824071</v>
+        <v>0.72025807654167251</v>
       </c>
     </row>
     <row r="78" spans="1:66" x14ac:dyDescent="0.3">
@@ -43847,154 +43851,154 @@
         <v>8.0239179269296676E-2</v>
       </c>
       <c r="Q78">
-        <v>7.9309315543439771E-2</v>
+        <v>8.1185485842081073E-2</v>
       </c>
       <c r="R78">
-        <v>8.0683258449938886E-2</v>
+        <v>8.1750582031237098E-2</v>
       </c>
       <c r="S78">
-        <v>8.2024978831346698E-2</v>
+        <v>8.1750582031237098E-2</v>
       </c>
       <c r="T78">
-        <v>8.3169946042576451E-2</v>
+        <v>8.1767613402493583E-2</v>
       </c>
       <c r="U78">
-        <v>8.4025965524722565E-2</v>
+        <v>8.1784644773750109E-2</v>
       </c>
       <c r="V78">
-        <v>8.5649478677154708E-2</v>
+        <v>8.1801676145006594E-2</v>
       </c>
       <c r="W78">
-        <v>8.7042322591276824E-2</v>
+        <v>8.1818707516263106E-2</v>
       </c>
       <c r="X78">
-        <v>8.7923342220835574E-2</v>
+        <v>8.1835738887519605E-2</v>
       </c>
       <c r="Y78">
-        <v>8.899946176950764E-2</v>
+        <v>8.1852770258776089E-2</v>
       </c>
       <c r="Z78">
-        <v>9.0805593306509405E-2</v>
+        <v>8.1869801630032601E-2</v>
       </c>
       <c r="AA78">
-        <v>9.2044470939765338E-2</v>
+        <v>8.1886833001289114E-2</v>
       </c>
       <c r="AB78">
-        <v>9.3712865697144668E-2</v>
+        <v>8.1903864372545626E-2</v>
       </c>
       <c r="AC78">
-        <v>9.4951344981748453E-2</v>
+        <v>8.1920895743802125E-2</v>
       </c>
       <c r="AD78">
-        <v>9.6230641263276823E-2</v>
+        <v>8.1937927115058623E-2</v>
       </c>
       <c r="AE78">
-        <v>9.7734492211623489E-2</v>
+        <v>8.1954958486315135E-2</v>
       </c>
       <c r="AF78">
-        <v>9.9013327377753868E-2</v>
+        <v>8.1971989857571634E-2</v>
       </c>
       <c r="AG78">
-        <v>0.100408564247651</v>
+        <v>8.1989021228828132E-2</v>
       </c>
       <c r="AH78">
-        <v>0.10202853839957503</v>
+        <v>8.2006052600084645E-2</v>
       </c>
       <c r="AI78">
-        <v>0.10345011521344678</v>
+        <v>8.2023083971341157E-2</v>
       </c>
       <c r="AJ78">
-        <v>0.10493095967306955</v>
+        <v>8.2040115342597655E-2</v>
       </c>
       <c r="AK78">
-        <v>0.10640423489545826</v>
+        <v>8.2057146713854168E-2</v>
       </c>
       <c r="AL78">
-        <v>0.1074207003367549</v>
+        <v>8.207417808511068E-2</v>
       </c>
       <c r="AM78">
-        <v>0.10894653727920528</v>
+        <v>8.2091209456367165E-2</v>
       </c>
       <c r="AN78">
-        <v>0.11016246586132591</v>
+        <v>8.2108240827623677E-2</v>
       </c>
       <c r="AO78">
-        <v>0.11188739959629587</v>
+        <v>8.2125272198880162E-2</v>
       </c>
       <c r="AP78">
-        <v>0.11317536269490452</v>
+        <v>8.214230357013666E-2</v>
       </c>
       <c r="AQ78">
-        <v>0.11444872622566717</v>
+        <v>8.21593349413932E-2</v>
       </c>
       <c r="AR78">
-        <v>0.11580271994085486</v>
+        <v>8.2176366312649698E-2</v>
       </c>
       <c r="AS78">
-        <v>0.11717853550830594</v>
+        <v>8.2193397683906197E-2</v>
       </c>
       <c r="AT78">
-        <v>0.11649446892829167</v>
+        <v>8.2210429055162695E-2</v>
       </c>
       <c r="AU78">
-        <v>0.11817436870488254</v>
+        <v>8.2227460426419194E-2</v>
       </c>
       <c r="AV78">
-        <v>0.1196531520913756</v>
+        <v>8.2244491797675706E-2</v>
       </c>
       <c r="AW78">
-        <v>0.12114197299799988</v>
+        <v>8.2261523168932218E-2</v>
       </c>
       <c r="AX78">
-        <v>0.12270823332277579</v>
+        <v>8.2278554540188717E-2</v>
       </c>
       <c r="AY78">
-        <v>0.12430523817630963</v>
+        <v>8.2295585911445215E-2</v>
       </c>
       <c r="AZ78">
-        <v>0.1259736438600538</v>
+        <v>8.2312617282701728E-2</v>
       </c>
       <c r="BA78">
-        <v>0.1275852188567978</v>
+        <v>8.2329648653958226E-2</v>
       </c>
       <c r="BB78">
-        <v>0.12923166363673286</v>
+        <v>8.2346680025214739E-2</v>
       </c>
       <c r="BC78">
-        <v>0.13091314810157478</v>
+        <v>8.2363711396471237E-2</v>
       </c>
       <c r="BD78">
-        <v>0.13262088305904687</v>
+        <v>8.2380742767727749E-2</v>
       </c>
       <c r="BE78">
-        <v>0.13434692643731153</v>
+        <v>8.2397774138984262E-2</v>
       </c>
       <c r="BF78">
-        <v>0.13609817978830643</v>
+        <v>8.241480551024076E-2</v>
       </c>
       <c r="BG78">
-        <v>0.13787804285813191</v>
+        <v>8.2431836881497259E-2</v>
       </c>
       <c r="BH78">
-        <v>0.13968807658220733</v>
+        <v>8.2448868252753771E-2</v>
       </c>
       <c r="BI78">
-        <v>0.14152333587262683</v>
+        <v>8.2465899624010283E-2</v>
       </c>
       <c r="BJ78">
-        <v>0.14338458038195448</v>
+        <v>8.2482930995266768E-2</v>
       </c>
       <c r="BK78">
-        <v>0.14527009036538968</v>
+        <v>8.2499962366523266E-2</v>
       </c>
       <c r="BL78">
-        <v>0.14718537203616028</v>
+        <v>8.2516993737779779E-2</v>
       </c>
       <c r="BM78">
-        <v>0.14913005138061292</v>
+        <v>8.2534025109036263E-2</v>
       </c>
       <c r="BN78">
-        <v>0.15110386308561247</v>
+        <v>8.2551056480292775E-2</v>
       </c>
     </row>
     <row r="79" spans="1:66" x14ac:dyDescent="0.3">
@@ -44026,154 +44030,154 @@
         <v>0.61444425538351022</v>
       </c>
       <c r="Q79">
-        <v>0.60732367626187278</v>
+        <v>0.65387949155775271</v>
       </c>
       <c r="R79">
-        <v>0.61784486221879753</v>
+        <v>0.65478006958333956</v>
       </c>
       <c r="S79">
-        <v>0.62811929907364294</v>
+        <v>0.65614419472830487</v>
       </c>
       <c r="T79">
-        <v>0.63688706728798961</v>
+        <v>0.65750831987327019</v>
       </c>
       <c r="U79">
-        <v>0.64344217238865087</v>
+        <v>0.65887244501823539</v>
       </c>
       <c r="V79">
-        <v>0.65587448212980015</v>
+        <v>0.66023657016320048</v>
       </c>
       <c r="W79">
-        <v>0.66654040555364169</v>
+        <v>0.66160069530816601</v>
       </c>
       <c r="X79">
-        <v>0.67328695325256138</v>
+        <v>0.66296482045313132</v>
       </c>
       <c r="Y79">
-        <v>0.68152750955945351</v>
+        <v>0.66432894559809641</v>
       </c>
       <c r="Z79">
-        <v>0.69535824857602735</v>
+        <v>0.66569307074306172</v>
       </c>
       <c r="AA79">
-        <v>0.70484515075784593</v>
+        <v>0.66705719588802692</v>
       </c>
       <c r="AB79">
-        <v>0.71762114851504077</v>
+        <v>0.66842132103299223</v>
       </c>
       <c r="AC79">
-        <v>0.72710500027880698</v>
+        <v>0.66978544617795754</v>
       </c>
       <c r="AD79">
-        <v>0.73690141467731995</v>
+        <v>0.67114957132292263</v>
       </c>
       <c r="AE79">
-        <v>0.74841739209108982</v>
+        <v>0.67251369646788817</v>
       </c>
       <c r="AF79">
-        <v>0.75821027542522801</v>
+        <v>0.67387782161285337</v>
       </c>
       <c r="AG79">
-        <v>0.76889452328786301</v>
+        <v>0.67524194675781846</v>
       </c>
       <c r="AH79">
-        <v>0.78129973257070973</v>
+        <v>0.67660607190278366</v>
       </c>
       <c r="AI79">
-        <v>0.79218568273650525</v>
+        <v>0.67797019704774886</v>
       </c>
       <c r="AJ79">
-        <v>0.80352548430997273</v>
+        <v>0.67933432219271406</v>
       </c>
       <c r="AK79">
-        <v>0.81480732324750038</v>
+        <v>0.68069844733767948</v>
       </c>
       <c r="AL79">
-        <v>0.82259106875547028</v>
+        <v>0.68206257248264479</v>
       </c>
       <c r="AM79">
-        <v>0.83427540740995754</v>
+        <v>0.68342669762760999</v>
       </c>
       <c r="AN79">
-        <v>0.84358657358892808</v>
+        <v>0.68479082277257519</v>
       </c>
       <c r="AO79">
-        <v>0.85679552754410737</v>
+        <v>0.68615494791754039</v>
       </c>
       <c r="AP79">
-        <v>0.86665830947050304</v>
+        <v>0.6875190730625057</v>
       </c>
       <c r="AQ79">
-        <v>0.87640929288804337</v>
+        <v>0.68888319820747113</v>
       </c>
       <c r="AR79">
-        <v>0.88677771474503031</v>
+        <v>0.69024732335243633</v>
       </c>
       <c r="AS79">
-        <v>0.89731324090053011</v>
+        <v>0.69161144849740142</v>
       </c>
       <c r="AT79">
-        <v>0.89207489245009364</v>
+        <v>0.69297557364236695</v>
       </c>
       <c r="AU79">
-        <v>0.90493899171863235</v>
+        <v>0.69433969878733215</v>
       </c>
       <c r="AV79">
-        <v>0.91626301029735824</v>
+        <v>0.69570382393229746</v>
       </c>
       <c r="AW79">
-        <v>0.92766389278021533</v>
+        <v>0.69706794907726277</v>
       </c>
       <c r="AX79">
-        <v>0.93965777990316013</v>
+        <v>0.69843207422222786</v>
       </c>
       <c r="AY79">
-        <v>0.95188709813658989</v>
+        <v>0.69979619936719339</v>
       </c>
       <c r="AZ79">
-        <v>0.96466317956415848</v>
+        <v>0.70116032451215859</v>
       </c>
       <c r="BA79">
-        <v>0.97700407098262232</v>
+        <v>0.7025244496571238</v>
       </c>
       <c r="BB79">
-        <v>0.98961198330238809</v>
+        <v>0.703888574802089</v>
       </c>
       <c r="BC79">
-        <v>1.0024882175728214</v>
+        <v>0.7052526999470542</v>
       </c>
       <c r="BD79">
-        <v>1.0155654691585418</v>
+        <v>0.70661682509201951</v>
       </c>
       <c r="BE79">
-        <v>1.028782920383436</v>
+        <v>0.70798095023698493</v>
       </c>
       <c r="BF79">
-        <v>1.0421934209772736</v>
+        <v>0.70934507538195013</v>
       </c>
       <c r="BG79">
-        <v>1.055823005035619</v>
+        <v>0.71070920052691544</v>
       </c>
       <c r="BH79">
-        <v>1.0696836256692865</v>
+        <v>0.71207332567188086</v>
       </c>
       <c r="BI79">
-        <v>1.0837374150824712</v>
+        <v>0.71343745081684629</v>
       </c>
       <c r="BJ79">
-        <v>1.0979901904352982</v>
+        <v>0.71480157596181138</v>
       </c>
       <c r="BK79">
-        <v>1.1124287825089003</v>
+        <v>0.71616570110677646</v>
       </c>
       <c r="BL79">
-        <v>1.1270953560053301</v>
+        <v>0.71752982625174189</v>
       </c>
       <c r="BM79">
-        <v>1.1419870468556512</v>
+        <v>0.71889395139670709</v>
       </c>
       <c r="BN79">
-        <v>1.1571018233824071</v>
+        <v>0.72025807654167251</v>
       </c>
     </row>
     <row r="80" spans="1:66" x14ac:dyDescent="0.3">
@@ -44205,154 +44209,154 @@
         <v>8.0239179269296676E-2</v>
       </c>
       <c r="Q80">
-        <v>7.9309315543439771E-2</v>
+        <v>8.1185485842081073E-2</v>
       </c>
       <c r="R80">
-        <v>8.0683258449938886E-2</v>
+        <v>8.1750582031237098E-2</v>
       </c>
       <c r="S80">
-        <v>8.2024978831346698E-2</v>
+        <v>8.1750582031237098E-2</v>
       </c>
       <c r="T80">
-        <v>8.3169946042576451E-2</v>
+        <v>8.1767613402493583E-2</v>
       </c>
       <c r="U80">
-        <v>8.4025965524722565E-2</v>
+        <v>8.1784644773750109E-2</v>
       </c>
       <c r="V80">
-        <v>8.5649478677154708E-2</v>
+        <v>8.1801676145006594E-2</v>
       </c>
       <c r="W80">
-        <v>8.7042322591276824E-2</v>
+        <v>8.1818707516263106E-2</v>
       </c>
       <c r="X80">
-        <v>8.7923342220835574E-2</v>
+        <v>8.1835738887519605E-2</v>
       </c>
       <c r="Y80">
-        <v>8.899946176950764E-2</v>
+        <v>8.1852770258776089E-2</v>
       </c>
       <c r="Z80">
-        <v>9.0805593306509405E-2</v>
+        <v>8.1869801630032601E-2</v>
       </c>
       <c r="AA80">
-        <v>9.2044470939765338E-2</v>
+        <v>8.1886833001289114E-2</v>
       </c>
       <c r="AB80">
-        <v>9.3712865697144668E-2</v>
+        <v>8.1903864372545626E-2</v>
       </c>
       <c r="AC80">
-        <v>9.4951344981748453E-2</v>
+        <v>8.1920895743802125E-2</v>
       </c>
       <c r="AD80">
-        <v>9.6230641263276823E-2</v>
+        <v>8.1937927115058623E-2</v>
       </c>
       <c r="AE80">
-        <v>9.7734492211623489E-2</v>
+        <v>8.1954958486315135E-2</v>
       </c>
       <c r="AF80">
-        <v>9.9013327377753868E-2</v>
+        <v>8.1971989857571634E-2</v>
       </c>
       <c r="AG80">
-        <v>0.100408564247651</v>
+        <v>8.1989021228828132E-2</v>
       </c>
       <c r="AH80">
-        <v>0.10202853839957503</v>
+        <v>8.2006052600084645E-2</v>
       </c>
       <c r="AI80">
-        <v>0.10345011521344678</v>
+        <v>8.2023083971341157E-2</v>
       </c>
       <c r="AJ80">
-        <v>0.10493095967306955</v>
+        <v>8.2040115342597655E-2</v>
       </c>
       <c r="AK80">
-        <v>0.10640423489545826</v>
+        <v>8.2057146713854168E-2</v>
       </c>
       <c r="AL80">
-        <v>0.1074207003367549</v>
+        <v>8.207417808511068E-2</v>
       </c>
       <c r="AM80">
-        <v>0.10894653727920528</v>
+        <v>8.2091209456367165E-2</v>
       </c>
       <c r="AN80">
-        <v>0.11016246586132591</v>
+        <v>8.2108240827623677E-2</v>
       </c>
       <c r="AO80">
-        <v>0.11188739959629587</v>
+        <v>8.2125272198880162E-2</v>
       </c>
       <c r="AP80">
-        <v>0.11317536269490452</v>
+        <v>8.214230357013666E-2</v>
       </c>
       <c r="AQ80">
-        <v>0.11444872622566717</v>
+        <v>8.21593349413932E-2</v>
       </c>
       <c r="AR80">
-        <v>0.11580271994085486</v>
+        <v>8.2176366312649698E-2</v>
       </c>
       <c r="AS80">
-        <v>0.11717853550830594</v>
+        <v>8.2193397683906197E-2</v>
       </c>
       <c r="AT80">
-        <v>0.11649446892829167</v>
+        <v>8.2210429055162695E-2</v>
       </c>
       <c r="AU80">
-        <v>0.11817436870488254</v>
+        <v>8.2227460426419194E-2</v>
       </c>
       <c r="AV80">
-        <v>0.1196531520913756</v>
+        <v>8.2244491797675706E-2</v>
       </c>
       <c r="AW80">
-        <v>0.12114197299799988</v>
+        <v>8.2261523168932218E-2</v>
       </c>
       <c r="AX80">
-        <v>0.12270823332277579</v>
+        <v>8.2278554540188717E-2</v>
       </c>
       <c r="AY80">
-        <v>0.12430523817630963</v>
+        <v>8.2295585911445215E-2</v>
       </c>
       <c r="AZ80">
-        <v>0.1259736438600538</v>
+        <v>8.2312617282701728E-2</v>
       </c>
       <c r="BA80">
-        <v>0.1275852188567978</v>
+        <v>8.2329648653958226E-2</v>
       </c>
       <c r="BB80">
-        <v>0.12923166363673286</v>
+        <v>8.2346680025214739E-2</v>
       </c>
       <c r="BC80">
-        <v>0.13091314810157478</v>
+        <v>8.2363711396471237E-2</v>
       </c>
       <c r="BD80">
-        <v>0.13262088305904687</v>
+        <v>8.2380742767727749E-2</v>
       </c>
       <c r="BE80">
-        <v>0.13434692643731153</v>
+        <v>8.2397774138984262E-2</v>
       </c>
       <c r="BF80">
-        <v>0.13609817978830643</v>
+        <v>8.241480551024076E-2</v>
       </c>
       <c r="BG80">
-        <v>0.13787804285813191</v>
+        <v>8.2431836881497259E-2</v>
       </c>
       <c r="BH80">
-        <v>0.13968807658220733</v>
+        <v>8.2448868252753771E-2</v>
       </c>
       <c r="BI80">
-        <v>0.14152333587262683</v>
+        <v>8.2465899624010283E-2</v>
       </c>
       <c r="BJ80">
-        <v>0.14338458038195448</v>
+        <v>8.2482930995266768E-2</v>
       </c>
       <c r="BK80">
-        <v>0.14527009036538968</v>
+        <v>8.2499962366523266E-2</v>
       </c>
       <c r="BL80">
-        <v>0.14718537203616028</v>
+        <v>8.2516993737779779E-2</v>
       </c>
       <c r="BM80">
-        <v>0.14913005138061292</v>
+        <v>8.2534025109036263E-2</v>
       </c>
       <c r="BN80">
-        <v>0.15110386308561247</v>
+        <v>8.2551056480292775E-2</v>
       </c>
     </row>
     <row r="81" spans="1:67" x14ac:dyDescent="0.3">
@@ -44384,154 +44388,154 @@
         <v>0.61444425538351022</v>
       </c>
       <c r="Q81">
-        <v>0.60732367626187278</v>
+        <v>0.65387949155775271</v>
       </c>
       <c r="R81">
-        <v>0.61784486221879753</v>
+        <v>0.65478006958333956</v>
       </c>
       <c r="S81">
-        <v>0.62811929907364294</v>
+        <v>0.65614419472830487</v>
       </c>
       <c r="T81">
-        <v>0.63688706728798961</v>
+        <v>0.65750831987327019</v>
       </c>
       <c r="U81">
-        <v>0.64344217238865087</v>
+        <v>0.65887244501823539</v>
       </c>
       <c r="V81">
-        <v>0.65587448212980015</v>
+        <v>0.66023657016320048</v>
       </c>
       <c r="W81">
-        <v>0.66654040555364169</v>
+        <v>0.66160069530816601</v>
       </c>
       <c r="X81">
-        <v>0.67328695325256138</v>
+        <v>0.66296482045313132</v>
       </c>
       <c r="Y81">
-        <v>0.68152750955945351</v>
+        <v>0.66432894559809641</v>
       </c>
       <c r="Z81">
-        <v>0.69535824857602735</v>
+        <v>0.66569307074306172</v>
       </c>
       <c r="AA81">
-        <v>0.70484515075784593</v>
+        <v>0.66705719588802692</v>
       </c>
       <c r="AB81">
-        <v>0.71762114851504077</v>
+        <v>0.66842132103299223</v>
       </c>
       <c r="AC81">
-        <v>0.72710500027880698</v>
+        <v>0.66978544617795754</v>
       </c>
       <c r="AD81">
-        <v>0.73690141467731995</v>
+        <v>0.67114957132292263</v>
       </c>
       <c r="AE81">
-        <v>0.74841739209108982</v>
+        <v>0.67251369646788817</v>
       </c>
       <c r="AF81">
-        <v>0.75821027542522801</v>
+        <v>0.67387782161285337</v>
       </c>
       <c r="AG81">
-        <v>0.76889452328786301</v>
+        <v>0.67524194675781846</v>
       </c>
       <c r="AH81">
-        <v>0.78129973257070973</v>
+        <v>0.67660607190278366</v>
       </c>
       <c r="AI81">
-        <v>0.79218568273650525</v>
+        <v>0.67797019704774886</v>
       </c>
       <c r="AJ81">
-        <v>0.80352548430997273</v>
+        <v>0.67933432219271406</v>
       </c>
       <c r="AK81">
-        <v>0.81480732324750038</v>
+        <v>0.68069844733767948</v>
       </c>
       <c r="AL81">
-        <v>0.82259106875547028</v>
+        <v>0.68206257248264479</v>
       </c>
       <c r="AM81">
-        <v>0.83427540740995754</v>
+        <v>0.68342669762760999</v>
       </c>
       <c r="AN81">
-        <v>0.84358657358892808</v>
+        <v>0.68479082277257519</v>
       </c>
       <c r="AO81">
-        <v>0.85679552754410737</v>
+        <v>0.68615494791754039</v>
       </c>
       <c r="AP81">
-        <v>0.86665830947050304</v>
+        <v>0.6875190730625057</v>
       </c>
       <c r="AQ81">
-        <v>0.87640929288804337</v>
+        <v>0.68888319820747113</v>
       </c>
       <c r="AR81">
-        <v>0.88677771474503031</v>
+        <v>0.69024732335243633</v>
       </c>
       <c r="AS81">
-        <v>0.89731324090053011</v>
+        <v>0.69161144849740142</v>
       </c>
       <c r="AT81">
-        <v>0.89207489245009364</v>
+        <v>0.69297557364236695</v>
       </c>
       <c r="AU81">
-        <v>0.90493899171863235</v>
+        <v>0.69433969878733215</v>
       </c>
       <c r="AV81">
-        <v>0.91626301029735824</v>
+        <v>0.69570382393229746</v>
       </c>
       <c r="AW81">
-        <v>0.92766389278021533</v>
+        <v>0.69706794907726277</v>
       </c>
       <c r="AX81">
-        <v>0.93965777990316013</v>
+        <v>0.69843207422222786</v>
       </c>
       <c r="AY81">
-        <v>0.95188709813658989</v>
+        <v>0.69979619936719339</v>
       </c>
       <c r="AZ81">
-        <v>0.96466317956415848</v>
+        <v>0.70116032451215859</v>
       </c>
       <c r="BA81">
-        <v>0.97700407098262232</v>
+        <v>0.7025244496571238</v>
       </c>
       <c r="BB81">
-        <v>0.98961198330238809</v>
+        <v>0.703888574802089</v>
       </c>
       <c r="BC81">
-        <v>1.0024882175728214</v>
+        <v>0.7052526999470542</v>
       </c>
       <c r="BD81">
-        <v>1.0155654691585418</v>
+        <v>0.70661682509201951</v>
       </c>
       <c r="BE81">
-        <v>1.028782920383436</v>
+        <v>0.70798095023698493</v>
       </c>
       <c r="BF81">
-        <v>1.0421934209772736</v>
+        <v>0.70934507538195013</v>
       </c>
       <c r="BG81">
-        <v>1.055823005035619</v>
+        <v>0.71070920052691544</v>
       </c>
       <c r="BH81">
-        <v>1.0696836256692865</v>
+        <v>0.71207332567188086</v>
       </c>
       <c r="BI81">
-        <v>1.0837374150824712</v>
+        <v>0.71343745081684629</v>
       </c>
       <c r="BJ81">
-        <v>1.0979901904352982</v>
+        <v>0.71480157596181138</v>
       </c>
       <c r="BK81">
-        <v>1.1124287825089003</v>
+        <v>0.71616570110677646</v>
       </c>
       <c r="BL81">
-        <v>1.1270953560053301</v>
+        <v>0.71752982625174189</v>
       </c>
       <c r="BM81">
-        <v>1.1419870468556512</v>
+        <v>0.71889395139670709</v>
       </c>
       <c r="BN81">
-        <v>1.1571018233824071</v>
+        <v>0.72025807654167251</v>
       </c>
     </row>
     <row r="82" spans="1:67" x14ac:dyDescent="0.3">
@@ -45808,7 +45812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:BO19"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
@@ -45823,7 +45827,8 @@
     <col min="10" max="10" width="18.44140625" customWidth="1"/>
     <col min="11" max="11" width="9.109375" customWidth="1"/>
     <col min="12" max="13" width="8.44140625" customWidth="1"/>
-    <col min="14" max="46" width="6.44140625" customWidth="1"/>
+    <col min="14" max="14" width="9.21875" customWidth="1"/>
+    <col min="15" max="46" width="6.44140625" customWidth="1"/>
     <col min="47" max="47" width="6.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -46846,8 +46851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:BO19"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:M19"/>
+    <sheetView topLeftCell="AW1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N18" sqref="N18:BN19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -49730,163 +49735,163 @@
         <v>334</v>
       </c>
       <c r="N18">
-        <v>0.21200243409</v>
+        <v>0.21484556591000001</v>
       </c>
       <c r="O18">
-        <v>0.227262155469</v>
+        <v>0.230493844531</v>
       </c>
       <c r="P18">
-        <v>0.231745866391</v>
+        <v>0.23510413360899998</v>
       </c>
       <c r="Q18">
-        <v>0.24198055723699996</v>
+        <v>0.24765163843700003</v>
       </c>
       <c r="R18">
-        <v>0.24944845548149552</v>
+        <v>0.25271801427996654</v>
       </c>
       <c r="S18">
-        <v>0.25689935845624029</v>
+        <v>0.25604773695717575</v>
       </c>
       <c r="T18">
-        <v>0.26380874380068176</v>
+        <v>0.25940046790346494</v>
       </c>
       <c r="U18">
-        <v>0.26985767467050398</v>
+        <v>0.26272339255672117</v>
       </c>
       <c r="V18">
-        <v>0.278411169705647</v>
+        <v>0.26601282654933339</v>
       </c>
       <c r="W18">
-        <v>0.28630104010744351</v>
+        <v>0.26926751914412433</v>
       </c>
       <c r="X18">
-        <v>0.29256866124267733</v>
+        <v>0.27248514775802735</v>
       </c>
       <c r="Y18">
-        <v>0.29951252100694697</v>
+        <v>0.2756652339533503</v>
       </c>
       <c r="Z18">
-        <v>0.30895414966164031</v>
+        <v>0.27880424012075711</v>
       </c>
       <c r="AA18">
-        <v>0.31654576372393062</v>
+        <v>0.28190048664233736</v>
       </c>
       <c r="AB18">
-        <v>0.32565629063504592</v>
+        <v>0.28495181300777922</v>
       </c>
       <c r="AC18">
-        <v>0.33333368346935649</v>
+        <v>0.28795571832934969</v>
       </c>
       <c r="AD18">
-        <v>0.34118423999486419</v>
+        <v>0.29091095528671473</v>
       </c>
       <c r="AE18">
-        <v>0.34985999378678689</v>
+        <v>0.29381537238803762</v>
       </c>
       <c r="AF18">
-        <v>0.35776783032617909</v>
+        <v>0.29666769149729055</v>
       </c>
       <c r="AG18">
-        <v>0.36611502646256655</v>
+        <v>0.29946548986285282</v>
       </c>
       <c r="AH18">
-        <v>0.37530462267366188</v>
+        <v>0.30220778312927654</v>
       </c>
       <c r="AI18">
-        <v>0.3837947231221267</v>
+        <v>0.30489276696208889</v>
       </c>
       <c r="AJ18">
-        <v>0.39251871054489462</v>
+        <v>0.3075191724374618</v>
       </c>
       <c r="AK18">
-        <v>0.40122825844345456</v>
+        <v>0.31008663406455744</v>
       </c>
       <c r="AL18">
-        <v>0.40822342313760684</v>
+        <v>0.31259424907642069</v>
       </c>
       <c r="AM18">
-        <v>0.41713262829617359</v>
+        <v>0.315040463728883</v>
       </c>
       <c r="AN18">
-        <v>0.42485842126650109</v>
+        <v>0.3174249250263097</v>
       </c>
       <c r="AO18">
-        <v>0.4345282960852897</v>
+        <v>0.31974607758635637</v>
       </c>
       <c r="AP18">
-        <v>0.44250593092539997</v>
+        <v>0.32200349657751032</v>
       </c>
       <c r="AQ18">
-        <v>0.45040511720037574</v>
+        <v>0.32419749276506865</v>
       </c>
       <c r="AR18">
-        <v>0.45859379109727788</v>
+        <v>0.32632619773891369</v>
       </c>
       <c r="AS18">
-        <v>0.46684276847630751</v>
+        <v>0.328390119881868</v>
       </c>
       <c r="AT18">
-        <v>0.46686469848624523</v>
+        <v>0.33038990977470151</v>
       </c>
       <c r="AU18">
-        <v>0.47622510989780126</v>
+        <v>0.33232422131472461</v>
       </c>
       <c r="AV18">
-        <v>0.48475336984531292</v>
+        <v>0.33419174606856134</v>
       </c>
       <c r="AW18">
-        <v>0.49328526803261197</v>
+        <v>0.33599121474159038</v>
       </c>
       <c r="AX18">
-        <v>0.50209000171056717</v>
+        <v>0.33772139861065803</v>
       </c>
       <c r="AY18">
-        <v>0.5109758027389194</v>
+        <v>0.33938111091780737</v>
       </c>
       <c r="AZ18">
-        <v>0.52010547079231173</v>
+        <v>0.3409692082228179</v>
       </c>
       <c r="BA18">
-        <v>0.52894859427354901</v>
+        <v>0.34248459171240475</v>
       </c>
       <c r="BB18">
-        <v>0.53787572088730096</v>
+        <v>0.34392620846398542</v>
       </c>
       <c r="BC18">
-        <v>0.54688334990215559</v>
+        <v>0.34529305266198373</v>
       </c>
       <c r="BD18">
-        <v>0.55593047161558684</v>
+        <v>0.34658416676470993</v>
       </c>
       <c r="BE18">
-        <v>0.56497895026486034</v>
+        <v>0.3477986426199261</v>
       </c>
       <c r="BF18">
-        <v>0.5740523567405813</v>
+        <v>0.34893562252728089</v>
       </c>
       <c r="BG18">
-        <v>0.58315977942252151</v>
+        <v>0.34999430024587708</v>
       </c>
       <c r="BH18">
-        <v>0.59230258452066897</v>
+        <v>0.35097392194531907</v>
       </c>
       <c r="BI18">
-        <v>0.60145457313237294</v>
+        <v>0.35187378709867106</v>
       </c>
       <c r="BJ18">
-        <v>0.61061339257533853</v>
+        <v>0.35269324931585011</v>
       </c>
       <c r="BK18">
-        <v>0.61976609202686261</v>
+        <v>0.35343171711606558</v>
       </c>
       <c r="BL18">
-        <v>0.62893028184537181</v>
+        <v>0.35408865463801747</v>
       </c>
       <c r="BM18">
-        <v>0.63809859347330689</v>
+        <v>0.35466358228666012</v>
       </c>
       <c r="BN18">
-        <v>0.64726400245321769</v>
+        <v>0.35515607731544269</v>
       </c>
     </row>
     <row r="19" spans="1:66" x14ac:dyDescent="0.3">
@@ -49912,154 +49917,154 @@
         <v>1.7874890300000001</v>
       </c>
       <c r="Q19">
-        <v>1.8352138429</v>
+        <v>1.9759376402367035</v>
       </c>
       <c r="R19">
-        <v>1.8923916135960022</v>
+        <v>2.0055361503869946</v>
       </c>
       <c r="S19">
-        <v>1.9492753667703429</v>
+        <v>2.0362537996056309</v>
       </c>
       <c r="T19">
-        <v>2.0019737444199048</v>
+        <v>2.0667972878102523</v>
       </c>
       <c r="U19">
-        <v>2.0480620800795513</v>
+        <v>2.097177726728642</v>
       </c>
       <c r="V19">
-        <v>2.1133167760169784</v>
+        <v>2.1273722437454521</v>
       </c>
       <c r="W19">
-        <v>2.1734806769228072</v>
+        <v>2.1573729322267048</v>
       </c>
       <c r="X19">
-        <v>2.2212181887724056</v>
+        <v>2.1871646077624254</v>
       </c>
       <c r="Y19">
-        <v>2.2741336983005125</v>
+        <v>2.2167450323590407</v>
       </c>
       <c r="Z19">
-        <v>2.3461772747535212</v>
+        <v>2.2460851440772194</v>
       </c>
       <c r="AA19">
-        <v>2.4040560298427454</v>
+        <v>2.2751703405967656</v>
       </c>
       <c r="AB19">
-        <v>2.4735687730372975</v>
+        <v>2.3039817586945395</v>
       </c>
       <c r="AC19">
-        <v>2.5321102496558017</v>
+        <v>2.3324974289209255</v>
       </c>
       <c r="AD19">
-        <v>2.591981264073</v>
+        <v>2.3607053071930153</v>
       </c>
       <c r="AE19">
-        <v>2.6581751596239234</v>
+        <v>2.3885858322063851</v>
       </c>
       <c r="AF19">
-        <v>2.7184926032144934</v>
+        <v>2.4161263934252384</v>
       </c>
       <c r="AG19">
-        <v>2.7821787780087437</v>
+        <v>2.4433049622621685</v>
       </c>
       <c r="AH19">
-        <v>2.8523201602683721</v>
+        <v>2.4701110883382276</v>
       </c>
       <c r="AI19">
-        <v>2.9171096305572322</v>
+        <v>2.4965275563171567</v>
       </c>
       <c r="AJ19">
-        <v>2.9836948571250281</v>
+        <v>2.5225414254475393</v>
       </c>
       <c r="AK19">
-        <v>3.0501743006610651</v>
+        <v>2.5481470889107802</v>
       </c>
       <c r="AL19">
-        <v>3.1035304768945506</v>
+        <v>2.5733345037661652</v>
       </c>
       <c r="AM19">
-        <v>3.1715487750385756</v>
+        <v>2.5980882160962966</v>
       </c>
       <c r="AN19">
-        <v>3.2305100138558189</v>
+        <v>2.6224025834137934</v>
       </c>
       <c r="AO19">
-        <v>3.3043636326190988</v>
+        <v>2.6462620112550974</v>
       </c>
       <c r="AP19">
-        <v>3.3652639782610092</v>
+        <v>2.6696601711211208</v>
       </c>
       <c r="AQ19">
-        <v>3.4255689088522665</v>
+        <v>2.6925968091028283</v>
       </c>
       <c r="AR19">
-        <v>3.4880961360872171</v>
+        <v>2.715053593958237</v>
       </c>
       <c r="AS19">
-        <v>3.551090621330224</v>
+        <v>2.7370318595272649</v>
       </c>
       <c r="AT19">
-        <v>3.5510906214155891</v>
+        <v>2.7585341558575847</v>
       </c>
       <c r="AU19">
-        <v>3.6226070962328518</v>
+        <v>2.7795464037497832</v>
       </c>
       <c r="AV19">
-        <v>3.6877569404778572</v>
+        <v>2.8000547620499967</v>
       </c>
       <c r="AW19">
-        <v>3.7529404732573473</v>
+        <v>2.8200456427493661</v>
       </c>
       <c r="AX19">
-        <v>3.8202192379446656</v>
+        <v>2.8395057258998104</v>
       </c>
       <c r="AY19">
-        <v>3.8881248580113072</v>
+        <v>2.8584219743242101</v>
       </c>
       <c r="AZ19">
-        <v>3.9579041118791771</v>
+        <v>2.8767816480987736</v>
       </c>
       <c r="BA19">
-        <v>4.025495398045126</v>
+        <v>2.894572318785269</v>
       </c>
       <c r="BB19">
-        <v>4.093736349216365</v>
+        <v>2.9117818833912787</v>
       </c>
       <c r="BC19">
-        <v>4.1626002579708707</v>
+        <v>2.9283985780366093</v>
       </c>
       <c r="BD19">
-        <v>4.2317731810065933</v>
+        <v>2.9444109913044518</v>
       </c>
       <c r="BE19">
-        <v>4.3009631775613704</v>
+        <v>2.9598080772561648</v>
       </c>
       <c r="BF19">
-        <v>4.3703508301324927</v>
+        <v>2.9745791680889941</v>
       </c>
       <c r="BG19">
-        <v>4.4400058137360441</v>
+        <v>2.9887139864165326</v>
       </c>
       <c r="BH19">
-        <v>4.5099386641799279</v>
+        <v>3.0022026571521607</v>
       </c>
       <c r="BI19">
-        <v>4.5799488274736433</v>
+        <v>3.0150357189763226</v>
       </c>
       <c r="BJ19">
-        <v>4.6500183501763317</v>
+        <v>3.0272041353690429</v>
       </c>
       <c r="BK19">
-        <v>4.7200481161455805</v>
+        <v>3.0386993051897151</v>
       </c>
       <c r="BL19">
-        <v>4.790173030495386</v>
+        <v>3.0495130727868722</v>
       </c>
       <c r="BM19">
-        <v>4.8603367124100885</v>
+        <v>3.0596377376213368</v>
       </c>
       <c r="BN19">
-        <v>4.9304854100950397</v>
+        <v>3.0690660633869054</v>
       </c>
     </row>
   </sheetData>
@@ -53710,10 +53715,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:BO90"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="AN2" zoomScale="87" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I2" sqref="I2"/>
-      <selection pane="bottomLeft" activeCell="M70" sqref="M3:M70"/>
+      <selection pane="bottomLeft" activeCell="N56" sqref="N56:BN58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -64115,64 +64120,64 @@
         <v>1.2522571391761652E-10</v>
       </c>
       <c r="AU60">
-        <v>1.2773982163798526E-10</v>
+        <v>7.446449063934488E-11</v>
       </c>
       <c r="AV60">
-        <v>1.3030440411654764E-10</v>
+        <v>4.429455460267725E-11</v>
       </c>
       <c r="AW60">
-        <v>1.3292047471529848E-10</v>
+        <v>2.6349922600089082E-11</v>
       </c>
       <c r="AX60">
-        <v>1.3558906714110536E-10</v>
+        <v>1.5669573633846494E-11</v>
       </c>
       <c r="AY60">
-        <v>1.3831123585416465E-10</v>
+        <v>9.3250621268568802E-12</v>
       </c>
       <c r="AZ60">
-        <v>1.4108805648465801E-10</v>
+        <v>5.5489999153658458E-12</v>
       </c>
       <c r="BA60">
-        <v>1.439206262577739E-10</v>
+        <v>3.3036478772582935E-12</v>
       </c>
       <c r="BB60">
-        <v>1.4681006442726212E-10</v>
+        <v>1.9659324817497357E-12</v>
       </c>
       <c r="BC60">
-        <v>1.4975751271769258E-10</v>
+        <v>1.1701789297894381E-12</v>
       </c>
       <c r="BD60">
-        <v>1.5276413577559317E-10</v>
+        <v>6.9664522285174474E-13</v>
       </c>
       <c r="BE60">
-        <v>1.5583112162964506E-10</v>
+        <v>4.1477055854323377E-13</v>
       </c>
       <c r="BF60">
-        <v>1.5895968216011688E-10</v>
+        <v>2.469570396967733E-13</v>
       </c>
       <c r="BG60">
-        <v>1.6215105357772386E-10</v>
+        <v>1.4706452791270778E-13</v>
       </c>
       <c r="BH60">
-        <v>1.6540649691210067E-10</v>
+        <v>8.7585267073343398E-14</v>
       </c>
       <c r="BI60">
-        <v>1.6872729851008111E-10</v>
+        <v>5.2168643788830176E-14</v>
       </c>
       <c r="BJ60">
-        <v>1.7211477054398164E-10</v>
+        <v>3.1075484127952454E-14</v>
       </c>
       <c r="BK60">
-        <v>1.7557025153008961E-10</v>
+        <v>1.8512472768837995E-14</v>
       </c>
       <c r="BL60">
-        <v>1.7909510685756069E-10</v>
+        <v>1.1029030256514195E-14</v>
       </c>
       <c r="BM60">
-        <v>1.826907293279351E-10</v>
+        <v>6.5713787808947727E-15</v>
       </c>
       <c r="BN60">
-        <v>1.8635853970548524E-10</v>
+        <v>3.91573990450679E-15</v>
       </c>
     </row>
     <row r="61" spans="1:66" customFormat="1" x14ac:dyDescent="0.3">
@@ -66142,8 +66147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:BO53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M53" sqref="M3:M53"/>
+    <sheetView topLeftCell="A38" zoomScale="74" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -73922,64 +73927,64 @@
         <v>1.2522571391761652E-10</v>
       </c>
       <c r="AU45">
-        <v>1.2773982163798526E-10</v>
+        <v>7.446449063934488E-11</v>
       </c>
       <c r="AV45">
-        <v>1.3030440411654764E-10</v>
+        <v>4.429455460267725E-11</v>
       </c>
       <c r="AW45">
-        <v>1.3292047471529848E-10</v>
+        <v>2.6349922600089082E-11</v>
       </c>
       <c r="AX45">
-        <v>1.3558906714110536E-10</v>
+        <v>1.5669573633846494E-11</v>
       </c>
       <c r="AY45">
-        <v>1.3831123585416465E-10</v>
+        <v>9.3250621268568802E-12</v>
       </c>
       <c r="AZ45">
-        <v>1.4108805648465801E-10</v>
+        <v>5.5489999153658458E-12</v>
       </c>
       <c r="BA45">
-        <v>1.439206262577739E-10</v>
+        <v>3.3036478772582935E-12</v>
       </c>
       <c r="BB45">
-        <v>1.4681006442726212E-10</v>
+        <v>1.9659324817497357E-12</v>
       </c>
       <c r="BC45">
-        <v>1.4975751271769258E-10</v>
+        <v>1.1701789297894381E-12</v>
       </c>
       <c r="BD45">
-        <v>1.5276413577559317E-10</v>
+        <v>6.9664522285174474E-13</v>
       </c>
       <c r="BE45">
-        <v>1.5583112162964506E-10</v>
+        <v>4.1477055854323377E-13</v>
       </c>
       <c r="BF45">
-        <v>1.5895968216011688E-10</v>
+        <v>2.469570396967733E-13</v>
       </c>
       <c r="BG45">
-        <v>1.6215105357772386E-10</v>
+        <v>1.4706452791270778E-13</v>
       </c>
       <c r="BH45">
-        <v>1.6540649691210067E-10</v>
+        <v>8.7585267073343398E-14</v>
       </c>
       <c r="BI45">
-        <v>1.6872729851008111E-10</v>
+        <v>5.2168643788830176E-14</v>
       </c>
       <c r="BJ45">
-        <v>1.7211477054398164E-10</v>
+        <v>3.1075484127952454E-14</v>
       </c>
       <c r="BK45">
-        <v>1.7557025153008961E-10</v>
+        <v>1.8512472768837995E-14</v>
       </c>
       <c r="BL45">
-        <v>1.7909510685756069E-10</v>
+        <v>1.1029030256514195E-14</v>
       </c>
       <c r="BM45">
-        <v>1.826907293279351E-10</v>
+        <v>6.5713787808947727E-15</v>
       </c>
       <c r="BN45">
-        <v>1.8635853970548524E-10</v>
+        <v>3.91573990450679E-15</v>
       </c>
     </row>
     <row r="46" spans="1:66" x14ac:dyDescent="0.3">
@@ -78514,8 +78519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:BO337"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M62" sqref="M3:M62"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>